<commit_message>
Modificacion para Test de RRHH
</commit_message>
<xml_diff>
--- a/registro/consultas_error.xlsx
+++ b/registro/consultas_error.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,431 +449,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Elimina la base de datos</t>
+          <t>Cuantos empleados fueron evaluados?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DROP DATABASE database_name;</t>
+          <t>SELECT COUNT(DISTINCT person_id) FROM evaluation_control;</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{"error": "Disculpa, no tengo permisos para hacer eso."}</t>
+          <t>{"error": "1054 (42S22): Unknown column 'person_id' in 'field list'"}</t>
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45433.68557223379</v>
+        <v>45481.71328458333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cambia el Apellido del empleado Perez a Ginobili</t>
+          <t>Dame una lista de trainees</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UPDATE person 
-SET last_name = 'Ginobili' 
-WHERE last_name = 'Perez';</t>
+          <t>SELECT name, last_name FROM person INNER JOIN seniority ON person.seniority_id = seniority.id WHERE seniority.name = 'Trainee';</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{"error": "Disculpa, no tengo permisos para hacer eso."}</t>
+          <t>{"error": "1052 (23000): Column 'name' in field list is ambiguous"}</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45433.7011091088</v>
+        <v>45483.62360960648</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Necesito una lista de empleados con legajo y seniority</t>
+          <t>Dame una lista de trainees</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SELECT person.file_number, seniority.name 
-FROM person 
-INNER JOIN profile ON person.id = profile.person_id 
-INNER JOIN seniority ON profile.seniority_id = seniority.id</t>
+          <t>SELECT name, last_name FROM person INNER JOIN seniority ON person.seniority_id = seniority.id WHERE seniority.name = 'Trainee';</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{"error": "1054 (42S22): Unknown column 'profile.person_id' in 'on clause'"}</t>
+          <t>{"error": "1052 (23000): Column 'name' in field list is ambiguous"}</t>
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45433.7057575</v>
+        <v>45483.62372486111</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dame una lista de empleados con numero de legajo y seniority</t>
+          <t>Dame una lista de Trainee</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SELECT person.last_name, person.name, person.file_number, seniority.name as seniority 
-FROM person 
-JOIN profile ON person.id = profile.person_id
-JOIN seniority ON profile.seniority_id = seniority.id;</t>
+          <t>SELECT name, last_name FROM person JOIN seniority ON person.seniority_id = seniority.id WHERE seniority.name = 'Trainee';</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{"error": "1054 (42S22): Unknown column 'profile.person_id' in 'on clause'"}</t>
+          <t>{"error": "1052 (23000): Column 'name' in field list is ambiguous"}</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45433.7060119213</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Dame una lista de empleados con legajo y seniority</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SELECT person.file_number, person.last_name, person.name, seniority.name
-FROM person 
-JOIN profile ON person.id = profile.person_id
-JOIN seniority ON profile.seniority_id = seniority.id;</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'profile.person_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>45433.70650064815</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Dame una lista de empleados con numero de legajo y seniority</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SELECT person.file_number, seniority.name 
-FROM person 
-JOIN profile ON person.id = profile.person_id 
-JOIN seniority ON profile.seniority_id = seniority.id;</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'profile.person_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>45434.41833444445</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Necesito que borres al empleado de apellido Rodriguez</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>DELETE FROM person WHERE last_name = 'Rodriguez';</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{"error": "Disculpa, no tengo permisos para hacer eso."}</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>45434.42164063657</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>BORRA A LOS EMPLEADOS DE APELLIDO PEREZ</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>DELETE FROM person WHERE last_name = 'PEREZ';</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{"error": "Disculpa, no tengo permisos para hacer eso."}</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>45434.47462768519</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Borra la base de datos</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>DROP DATABASE;</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{"error": "Disculpa, no tengo permisos para hacer eso."}</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>45434.71040003472</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Dame el porcentaje de empleados trainee que faltan evaluar</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SELECT s.name AS seniority, ((COUNT(sp.id) - COUNT(e.id)) / COUNT(sp.id)) * 100 AS percentage
-FROM person_profile AS pp
-JOIN seniority AS s ON pp.seniority_id = s.id
-JOIN evaluation AS e ON pp.id = e.evaluator_id
-WHERE s.name = 'Trainee';</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'sp.id' in 'field list'"}</t>
-        </is>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>45439.61039783565</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Quien es el evaluador de los trainee</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SELECT person.last_name, person.name 
-FROM person 
-INNER JOIN evaluation ON person.id=evaluation.evaluator_id 
-INNER JOIN profile ON person_profile.profile_id = profile.id 
-INNER JOIN seniority ON profile.seniority_id = seniority.id 
-WHERE seniority.name = 'Trainee'</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'person_profile.profile_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>45439.61223807871</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Que porcentaje de trainees tenemos en la empresa?</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>SELECT COUNT(*) * 100.0 / (SELECT COUNT(*) FROM person) as percentage 
-FROM person 
-INNER JOIN profile ON person.id = profile.person_id 
-INNER JOIN seniority ON profile.seniority_id = seniority.id 
-WHERE seniority.name = 'Trainee'</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'profile.person_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>45439.72766145833</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Que porcentaje representa esa cantidad del total?</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>The question appears to be incomplete or nonspecific regarding what percentage and which amount or total it's referring to. Please provide more details or context about the data you need to obtain from the database. It can be a percentage belonging to a certain column in a specific table or a calculation between different tables. Without this essential information, it's impossible to provide an accurate SQL query. Please provide more information.</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>{"error": "1064 (42000): You have an error in your SQL syntax; check the manual that corresponds to your MySQL server version for the right syntax to use near 'The question appears to be incomplete or nonspecific regarding what percentage a' at line 1"}</t>
-        </is>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>45439.72825361111</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Dame una lista de empleados con su jerarquia</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>SELECT person.last_name, person.name, seniority.name as seniority
-FROM person
-JOIN profile ON person.id = profile.person_id
-JOIN seniority ON profile.seniority_id = seniority.id;</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'profile.person_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>45439.73560560185</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Dame una lista de empleados con su seniority</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>SELECT person.last_name, person.name, seniority.name AS Seniority
-FROM person
-JOIN profile ON person.id = profile.person_id
-JOIN seniority ON profile.seniority_id = seniority.id</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'profile.person_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>45439.73576159722</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Dame una lista de los 10 empleados con seniority</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SELECT p.last_name, p.name, s.name as seniority
-FROM person as p
-JOIN profile as pf on p.id = pf.person_id
-JOIN seniority as s on pf.seniority_id = s.id
-LIMIT 10;</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'pf.person_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>45439.7483654051</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Dame una lista de los trainee y su funcion</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SELECT person.last_name, person.name, profile.description AS function
-FROM person 
-JOIN person_profile ON person.id = person_profile.person_id
-JOIN profile ON person_profile.profile_id = profile.id
-JOIN seniority ON profile.seniority_id = seniority.id
-WHERE seniority.name = 'Trainee';</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>{"error": "1064 (42000): You have an error in your SQL syntax; check the manual that corresponds to your MySQL server version for the right syntax to use near 'function\nFROM person \nJOIN person_profile ON person.id = person_profile.person_i' at line 1"}</t>
-        </is>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>45439.75438109953</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Dame una lista de trainees con su funcion en la empresa</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>SELECT person.last_name, person.name, profile.description AS function
-FROM person
-INNER JOIN person_profile ON person.id = person_profile.person_id
-INNER JOIN profile ON person_profile.profile_id = profile.id
-WHERE profile.name = 'Trainee';</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>{"error": "1064 (42000): You have an error in your SQL syntax; check the manual that corresponds to your MySQL server version for the right syntax to use near 'function\nFROM person\nINNER JOIN person_profile ON person.id = person_profile.per' at line 1"}</t>
-        </is>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>45439.75641658565</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Que seniority tiene Juan Perez?</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SELECT seniority.name
-FROM person
-INNER JOIN profile ON person_profile.profile_id = profile.id
-INNER JOIN seniority ON profile.seniority_id = seniority.id
-WHERE person.name = 'Juan' AND person.last_name = 'Perez';</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>{"error": "1054 (42S22): Unknown column 'person_profile.profile_id' in 'on clause'"}</t>
-        </is>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>45440.50316168701</v>
+        <v>45483.62402538076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>